<commit_message>
added hedgerow variable for Belgium funding
</commit_message>
<xml_diff>
--- a/data/funding_data1.xlsx
+++ b/data/funding_data1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\data\Shiny_UI_App\funding_dynamic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43AB330-2CE3-4127-A9C1-6DA463F6A945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3AABB5-5E2F-4676-931F-1DA316F969E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="247">
   <si>
     <t>Country</t>
   </si>
@@ -1042,6 +1042,9 @@
   </si>
   <si>
     <t>funding_onetime_percentage_initial_cost_schemes_c</t>
+  </si>
+  <si>
+    <t>funding_onetime_per_m_hedgerow_schemes_c</t>
   </si>
 </sst>
 </file>
@@ -1646,9 +1649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1725,7 +1728,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.2">
+    <row r="5" spans="1:10" ht="28.8">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>237</v>
@@ -1984,7 +1987,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8">
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8">
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8">
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>69</v>
       </c>
@@ -2122,7 +2125,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:10" ht="28.8">
+    <row r="17" spans="1:10">
       <c r="A17" s="3" t="s">
         <v>69</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="43.2">
+    <row r="18" spans="1:10" ht="28.8">
       <c r="A18" s="3" t="s">
         <v>69</v>
       </c>
@@ -2176,7 +2179,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="28.8">
+    <row r="19" spans="1:10" ht="15.6">
       <c r="A19" s="3" t="s">
         <v>69</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8">
+    <row r="20" spans="1:10" ht="15.6">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="28.8">
+    <row r="21" spans="1:10" ht="15.6">
       <c r="A21" s="3" t="s">
         <v>69</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28.8">
+    <row r="22" spans="1:10" ht="15.6">
       <c r="A22" s="3" t="s">
         <v>69</v>
       </c>
@@ -2282,7 +2285,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="38"/>
     </row>
-    <row r="23" spans="1:10" ht="28.8">
+    <row r="23" spans="1:10" ht="15.6">
       <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
@@ -2340,7 +2343,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.8">
+    <row r="25" spans="1:10" ht="15.6">
       <c r="A25" s="3" t="s">
         <v>76</v>
       </c>
@@ -2369,7 +2372,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.8">
+    <row r="26" spans="1:10" ht="15.6">
       <c r="A26" s="3" t="s">
         <v>76</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8">
+    <row r="27" spans="1:10" ht="15.6">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="28.8">
+    <row r="29" spans="1:10" ht="15.6">
       <c r="A29" s="3" t="s">
         <v>76</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="28.8">
+    <row r="30" spans="1:10">
       <c r="A30" s="11" t="s">
         <v>90</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28.8">
+    <row r="31" spans="1:10">
       <c r="A31" s="11" t="s">
         <v>90</v>
       </c>
@@ -2572,7 +2575,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="28.8">
+    <row r="33" spans="1:10">
       <c r="A33" s="11" t="s">
         <v>90</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="28.8">
+    <row r="35" spans="1:10">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.8">
+    <row r="36" spans="1:10">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -2684,7 +2687,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="28.8">
+    <row r="37" spans="1:10">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="28.8">
+    <row r="40" spans="1:10">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
@@ -2796,7 +2799,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="28.8">
+    <row r="41" spans="1:10">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="37" customFormat="1" ht="28.8">
+    <row r="43" spans="1:10" s="37" customFormat="1">
       <c r="A43" s="34" t="s">
         <v>4</v>
       </c>
@@ -2883,7 +2886,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="28.8">
+    <row r="44" spans="1:10">
       <c r="A44" s="3" t="s">
         <v>4</v>
       </c>
@@ -2910,7 +2913,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="28.8">
+    <row r="45" spans="1:10">
       <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="28.8">
+    <row r="46" spans="1:10">
       <c r="A46" s="3" t="s">
         <v>4</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="28.8">
+    <row r="47" spans="1:10">
       <c r="A47" s="3" t="s">
         <v>4</v>
       </c>
@@ -2991,7 +2994,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28.8">
+    <row r="48" spans="1:10">
       <c r="A48" s="3" t="s">
         <v>4</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="28.8">
+    <row r="49" spans="1:10">
       <c r="A49" s="3" t="s">
         <v>4</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="28.8">
+    <row r="52" spans="1:10">
       <c r="A52" s="3" t="s">
         <v>5</v>
       </c>
@@ -3175,7 +3178,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="28.8">
+    <row r="55" spans="1:10">
       <c r="A55" s="3" t="s">
         <v>5</v>
       </c>
@@ -3201,7 +3204,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="28.8">
+    <row r="56" spans="1:10">
       <c r="A56" s="3" t="s">
         <v>5</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="28.8">
+    <row r="57" spans="1:10">
       <c r="A57" s="3" t="s">
         <v>5</v>
       </c>
@@ -3253,7 +3256,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="28.8">
+    <row r="58" spans="1:10">
       <c r="A58" s="3" t="s">
         <v>5</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="28.8">
+    <row r="62" spans="1:10">
       <c r="A62" s="3" t="s">
         <v>5</v>
       </c>
@@ -3381,7 +3384,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="28.8">
+    <row r="63" spans="1:10">
       <c r="A63" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
minor edits + units added
</commit_message>
<xml_diff>
--- a/data/funding_data1.xlsx
+++ b/data/funding_data1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Apple_Agroforestry\Apple_Agroforestry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\Project_report\Deliverables\D4.3_Model_Comparison\Fruit_Honey_Agroforestry\Fruit_Honey_Agroforestry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3AABB5-5E2F-4676-931F-1DA316F969E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F330A6C9-1195-4C71-8A9B-D53288B2020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -62,6 +63,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -78,6 +80,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -94,6 +97,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -110,6 +114,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -126,6 +131,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Supported by Govt Forestry Commission Agroforestry Woodland Officers
@@ -140,6 +146,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Free bespoke design advice from Woodland Trust agroforestry advisors
@@ -164,6 +171,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -180,6 +188,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -196,6 +205,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -212,6 +222,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -228,6 +239,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -244,6 +256,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -260,6 +273,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Supported by Govt Forestry Commission Agroforestry Woodland Officers
@@ -274,6 +288,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Free bespoke design advice from Woodland Trust agroforestry advisors
@@ -286,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="248">
   <si>
     <t>Country</t>
   </si>
@@ -866,6 +881,7 @@
         <sz val="11"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Aanplantsubsidie voor boslandbouwsystemen (agroforestry) | Landbouw en Zeevisserij (vlaanderen.be)</t>
     </r>
@@ -877,6 +893,7 @@
         <sz val="11"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>VLIF Niet-productieve investeringen voor milieu- en klimaatdoelen | Landbouw en Zeevisserij (vlaanderen.be)</t>
     </r>
@@ -1045,6 +1062,9 @@
   </si>
   <si>
     <t>funding_onetime_per_m_hedgerow_schemes_c</t>
+  </si>
+  <si>
+    <t>Planting subsidy for new agroforestry plots (as per Agromilieu Klimaatmaatregelen (AMKM))</t>
   </si>
 </sst>
 </file>
@@ -1084,12 +1104,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1100,6 +1122,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1107,6 +1130,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1143,12 +1167,14 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1651,7 +1677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1712,8 +1738,8 @@
       <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>186</v>
+      <c r="E2" s="42" t="s">
+        <v>247</v>
       </c>
       <c r="F2" s="6">
         <v>0.75</v>

</xml_diff>